<commit_message>
refactored app to used property reflexion
</commit_message>
<xml_diff>
--- a/Planning Report/application sprint planner sprint5 03.02.20.xlsx
+++ b/Planning Report/application sprint planner sprint5 03.02.20.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68A1403E-51CF-482A-8406-E04D22DBB88E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBEA7F44-23B1-4A6F-A8A4-9E310C899482}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5520" yWindow="1050" windowWidth="21600" windowHeight="11385" tabRatio="415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1636,6 +1636,12 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1664,7 +1670,35 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="2" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="2" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -3648,40 +3682,6 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="2" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <border>
         <left style="thin">
           <color theme="0" tint="-0.24994659260841701"/>
@@ -4003,10 +4003,10 @@
     <filterColumn colId="6" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Milestone description" dataDxfId="106" totalsRowDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{C2AA6DD8-DBD1-4E89-A1EF-3287225D3E74}" name="Required" dataDxfId="105" totalsRowDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Category" dataDxfId="104" totalsRowDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Estimated Duration" dataDxfId="103" totalsRowDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Milestone description" dataDxfId="9" totalsRowDxfId="8"/>
+    <tableColumn id="7" xr3:uid="{C2AA6DD8-DBD1-4E89-A1EF-3287225D3E74}" name="Required" dataDxfId="7" totalsRowDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Category" dataDxfId="5" totalsRowDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Estimated Duration" dataDxfId="3" totalsRowDxfId="2"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Progress"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Start" totalsRowDxfId="1" dataCellStyle="Date"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="No. Days" totalsRowDxfId="0" dataCellStyle="Comma [0]"/>
@@ -4286,8 +4286,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:BM190"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A177" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="E187" sqref="E187"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A138" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="D149" sqref="D149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -34375,7 +34375,7 @@
     </row>
     <row r="148" spans="1:65" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" s="15"/>
-      <c r="B148" s="41" t="s">
+      <c r="B148" s="62" t="s">
         <v>48</v>
       </c>
       <c r="C148" s="41"/>
@@ -41492,56 +41492,56 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J5:BM8 J186:BM187 J136:BM136 J154:BM154 J74:BM75 J10:BM10 J22:BM58 J61:BM70 J72:BM72 J78:BM121 J124:BM132">
-    <cfRule type="expression" dxfId="102" priority="250">
+    <cfRule type="expression" dxfId="106" priority="250">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:AN4">
-    <cfRule type="expression" dxfId="101" priority="256">
+    <cfRule type="expression" dxfId="105" priority="256">
       <formula>J$5&lt;=EOMONTH($J$5,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K4:BM4">
-    <cfRule type="expression" dxfId="100" priority="252">
+    <cfRule type="expression" dxfId="104" priority="252">
       <formula>AND(K$5&lt;=EOMONTH($J$5,2),K$5&gt;EOMONTH($J$5,0),K$5&gt;EOMONTH($J$5,1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:BM4">
-    <cfRule type="expression" dxfId="99" priority="251">
+    <cfRule type="expression" dxfId="103" priority="251">
       <formula>AND(J$5&lt;=EOMONTH($J$5,1),J$5&gt;EOMONTH($J$5,0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J8:BM8 J10:BM10 J22:BM123 J169:BM186 J135:BM163">
-    <cfRule type="expression" dxfId="98" priority="273" stopIfTrue="1">
+    <cfRule type="expression" dxfId="102" priority="273" stopIfTrue="1">
       <formula>AND($D8="Low risk",J$5&gt;=$G8,J$5&lt;=$G8+$H8-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="97" priority="292" stopIfTrue="1">
+    <cfRule type="expression" dxfId="101" priority="292" stopIfTrue="1">
       <formula>AND($D8="High risk",J$5&gt;=$G8,J$5&lt;=$G8+$H8-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="96" priority="310" stopIfTrue="1">
+    <cfRule type="expression" dxfId="100" priority="310" stopIfTrue="1">
       <formula>AND($D8="On track",J$5&gt;=$G8,J$5&lt;=$G8+$H8-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="95" priority="311" stopIfTrue="1">
+    <cfRule type="expression" dxfId="99" priority="311" stopIfTrue="1">
       <formula>AND($D8="Med risk",J$5&gt;=$G8,J$5&lt;=$G8+$H8-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="94" priority="312" stopIfTrue="1">
+    <cfRule type="expression" dxfId="98" priority="312" stopIfTrue="1">
       <formula>AND(LEN($D8)=0,J$5&gt;=$G8,J$5&lt;=$G8+$H8-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J187:BM187">
-    <cfRule type="expression" dxfId="93" priority="320" stopIfTrue="1">
+    <cfRule type="expression" dxfId="97" priority="320" stopIfTrue="1">
       <formula>AND(#REF!="Low risk",J$5&gt;=#REF!,J$5&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="92" priority="321" stopIfTrue="1">
+    <cfRule type="expression" dxfId="96" priority="321" stopIfTrue="1">
       <formula>AND(#REF!="High risk",J$5&gt;=#REF!,J$5&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="91" priority="322" stopIfTrue="1">
+    <cfRule type="expression" dxfId="95" priority="322" stopIfTrue="1">
       <formula>AND(#REF!="On track",J$5&gt;=#REF!,J$5&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="90" priority="323" stopIfTrue="1">
+    <cfRule type="expression" dxfId="94" priority="323" stopIfTrue="1">
       <formula>AND(#REF!="Med risk",J$5&gt;=#REF!,J$5&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="89" priority="324" stopIfTrue="1">
+    <cfRule type="expression" dxfId="93" priority="324" stopIfTrue="1">
       <formula>AND(LEN(#REF!)=0,J$5&gt;=#REF!,J$5&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -41560,24 +41560,24 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J9:BM9">
-    <cfRule type="expression" dxfId="88" priority="241">
+    <cfRule type="expression" dxfId="92" priority="241">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J9:BM9">
-    <cfRule type="expression" dxfId="87" priority="243" stopIfTrue="1">
+    <cfRule type="expression" dxfId="91" priority="243" stopIfTrue="1">
       <formula>AND($D9="Low risk",J$5&gt;=$G9,J$5&lt;=$G9+$H9-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="86" priority="244" stopIfTrue="1">
+    <cfRule type="expression" dxfId="90" priority="244" stopIfTrue="1">
       <formula>AND($D9="High risk",J$5&gt;=$G9,J$5&lt;=$G9+$H9-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="85" priority="245" stopIfTrue="1">
+    <cfRule type="expression" dxfId="89" priority="245" stopIfTrue="1">
       <formula>AND($D9="On track",J$5&gt;=$G9,J$5&lt;=$G9+$H9-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="84" priority="246" stopIfTrue="1">
+    <cfRule type="expression" dxfId="88" priority="246" stopIfTrue="1">
       <formula>AND($D9="Med risk",J$5&gt;=$G9,J$5&lt;=$G9+$H9-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="83" priority="247" stopIfTrue="1">
+    <cfRule type="expression" dxfId="87" priority="247" stopIfTrue="1">
       <formula>AND(LEN($D9)=0,J$5&gt;=$G9,J$5&lt;=$G9+$H9-1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -41596,7 +41596,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J76:BM77">
-    <cfRule type="expression" dxfId="82" priority="225">
+    <cfRule type="expression" dxfId="86" priority="225">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -41615,7 +41615,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J123:GC123">
-    <cfRule type="expression" dxfId="81" priority="216">
+    <cfRule type="expression" dxfId="85" priority="216">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -41634,7 +41634,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J122:BM122">
-    <cfRule type="expression" dxfId="80" priority="209">
+    <cfRule type="expression" dxfId="84" priority="209">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -41653,7 +41653,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J59:BM60">
-    <cfRule type="expression" dxfId="79" priority="201">
+    <cfRule type="expression" dxfId="83" priority="201">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -41672,7 +41672,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J152:GC154 J157:GC157 J169:GC185 J137:GC150">
-    <cfRule type="expression" dxfId="78" priority="185">
+    <cfRule type="expression" dxfId="82" priority="185">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -41691,7 +41691,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J151:GC151">
-    <cfRule type="expression" dxfId="77" priority="177">
+    <cfRule type="expression" dxfId="81" priority="177">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -41710,7 +41710,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J134:GC135">
-    <cfRule type="expression" dxfId="76" priority="168">
+    <cfRule type="expression" dxfId="80" priority="168">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -41729,7 +41729,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J71:GC71">
-    <cfRule type="expression" dxfId="75" priority="160">
+    <cfRule type="expression" dxfId="79" priority="160">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -41748,7 +41748,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J155:GC156">
-    <cfRule type="expression" dxfId="74" priority="144">
+    <cfRule type="expression" dxfId="78" priority="144">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -41767,7 +41767,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J158:GC159">
-    <cfRule type="expression" dxfId="73" priority="136">
+    <cfRule type="expression" dxfId="77" priority="136">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -41786,7 +41786,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J162:GC162">
-    <cfRule type="expression" dxfId="72" priority="128">
+    <cfRule type="expression" dxfId="76" priority="128">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -41805,7 +41805,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J163:GC168">
-    <cfRule type="expression" dxfId="71" priority="120">
+    <cfRule type="expression" dxfId="75" priority="120">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -41824,7 +41824,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J73:BM73">
-    <cfRule type="expression" dxfId="70" priority="104">
+    <cfRule type="expression" dxfId="74" priority="104">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -41843,7 +41843,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J161:BM161">
-    <cfRule type="expression" dxfId="69" priority="96">
+    <cfRule type="expression" dxfId="73" priority="96">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -41862,7 +41862,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J133:BM133">
-    <cfRule type="expression" dxfId="68" priority="64">
+    <cfRule type="expression" dxfId="72" priority="64">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -41881,7 +41881,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J160:GC160">
-    <cfRule type="expression" dxfId="67" priority="72">
+    <cfRule type="expression" dxfId="71" priority="72">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -41900,24 +41900,24 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J11:BM11">
-    <cfRule type="expression" dxfId="66" priority="48">
+    <cfRule type="expression" dxfId="70" priority="48">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J11:BM11">
-    <cfRule type="expression" dxfId="65" priority="50" stopIfTrue="1">
+    <cfRule type="expression" dxfId="69" priority="50" stopIfTrue="1">
       <formula>AND($D11="Low risk",J$5&gt;=$G11,J$5&lt;=$G11+$H11-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="64" priority="51" stopIfTrue="1">
+    <cfRule type="expression" dxfId="68" priority="51" stopIfTrue="1">
       <formula>AND($D11="High risk",J$5&gt;=$G11,J$5&lt;=$G11+$H11-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="63" priority="52" stopIfTrue="1">
+    <cfRule type="expression" dxfId="67" priority="52" stopIfTrue="1">
       <formula>AND($D11="On track",J$5&gt;=$G11,J$5&lt;=$G11+$H11-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="62" priority="53" stopIfTrue="1">
+    <cfRule type="expression" dxfId="66" priority="53" stopIfTrue="1">
       <formula>AND($D11="Med risk",J$5&gt;=$G11,J$5&lt;=$G11+$H11-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="61" priority="54" stopIfTrue="1">
+    <cfRule type="expression" dxfId="65" priority="54" stopIfTrue="1">
       <formula>AND(LEN($D11)=0,J$5&gt;=$G11,J$5&lt;=$G11+$H11-1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -41936,24 +41936,24 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J12:BM14">
-    <cfRule type="expression" dxfId="60" priority="40">
+    <cfRule type="expression" dxfId="64" priority="40">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J12:BM14">
-    <cfRule type="expression" dxfId="59" priority="42" stopIfTrue="1">
+    <cfRule type="expression" dxfId="63" priority="42" stopIfTrue="1">
       <formula>AND($D12="Low risk",J$5&gt;=$G12,J$5&lt;=$G12+$H12-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="58" priority="43" stopIfTrue="1">
+    <cfRule type="expression" dxfId="62" priority="43" stopIfTrue="1">
       <formula>AND($D12="High risk",J$5&gt;=$G12,J$5&lt;=$G12+$H12-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="57" priority="44" stopIfTrue="1">
+    <cfRule type="expression" dxfId="61" priority="44" stopIfTrue="1">
       <formula>AND($D12="On track",J$5&gt;=$G12,J$5&lt;=$G12+$H12-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="56" priority="45" stopIfTrue="1">
+    <cfRule type="expression" dxfId="60" priority="45" stopIfTrue="1">
       <formula>AND($D12="Med risk",J$5&gt;=$G12,J$5&lt;=$G12+$H12-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="55" priority="46" stopIfTrue="1">
+    <cfRule type="expression" dxfId="59" priority="46" stopIfTrue="1">
       <formula>AND(LEN($D12)=0,J$5&gt;=$G12,J$5&lt;=$G12+$H12-1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -41972,24 +41972,24 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J15:BM15">
-    <cfRule type="expression" dxfId="54" priority="32">
+    <cfRule type="expression" dxfId="58" priority="32">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J15:BM15">
-    <cfRule type="expression" dxfId="53" priority="34" stopIfTrue="1">
+    <cfRule type="expression" dxfId="57" priority="34" stopIfTrue="1">
       <formula>AND($D15="Low risk",J$5&gt;=$G15,J$5&lt;=$G15+$H15-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="52" priority="35" stopIfTrue="1">
+    <cfRule type="expression" dxfId="56" priority="35" stopIfTrue="1">
       <formula>AND($D15="High risk",J$5&gt;=$G15,J$5&lt;=$G15+$H15-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="51" priority="36" stopIfTrue="1">
+    <cfRule type="expression" dxfId="55" priority="36" stopIfTrue="1">
       <formula>AND($D15="On track",J$5&gt;=$G15,J$5&lt;=$G15+$H15-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="50" priority="37" stopIfTrue="1">
+    <cfRule type="expression" dxfId="54" priority="37" stopIfTrue="1">
       <formula>AND($D15="Med risk",J$5&gt;=$G15,J$5&lt;=$G15+$H15-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="49" priority="38" stopIfTrue="1">
+    <cfRule type="expression" dxfId="53" priority="38" stopIfTrue="1">
       <formula>AND(LEN($D15)=0,J$5&gt;=$G15,J$5&lt;=$G15+$H15-1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -42008,46 +42008,46 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J16:BM18">
-    <cfRule type="expression" dxfId="48" priority="24">
+    <cfRule type="expression" dxfId="52" priority="24">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J16:BM18">
-    <cfRule type="expression" dxfId="47" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="51" priority="26" stopIfTrue="1">
       <formula>AND($D16="Low risk",J$5&gt;=$G16,J$5&lt;=$G16+$H16-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="46" priority="27" stopIfTrue="1">
+    <cfRule type="expression" dxfId="50" priority="27" stopIfTrue="1">
       <formula>AND($D16="High risk",J$5&gt;=$G16,J$5&lt;=$G16+$H16-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="45" priority="28" stopIfTrue="1">
+    <cfRule type="expression" dxfId="49" priority="28" stopIfTrue="1">
       <formula>AND($D16="On track",J$5&gt;=$G16,J$5&lt;=$G16+$H16-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="44" priority="29" stopIfTrue="1">
+    <cfRule type="expression" dxfId="48" priority="29" stopIfTrue="1">
       <formula>AND($D16="Med risk",J$5&gt;=$G16,J$5&lt;=$G16+$H16-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="43" priority="30" stopIfTrue="1">
+    <cfRule type="expression" dxfId="47" priority="30" stopIfTrue="1">
       <formula>AND(LEN($D16)=0,J$5&gt;=$G16,J$5&lt;=$G16+$H16-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J19:BM19">
-    <cfRule type="expression" dxfId="42" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="46" priority="19" stopIfTrue="1">
       <formula>AND($D19="Low risk",J$5&gt;=$G19,J$5&lt;=$G19+$H19-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="41" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="45" priority="20" stopIfTrue="1">
       <formula>AND($D19="High risk",J$5&gt;=$G19,J$5&lt;=$G19+$H19-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="44" priority="21" stopIfTrue="1">
       <formula>AND($D19="On track",J$5&gt;=$G19,J$5&lt;=$G19+$H19-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="39" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="43" priority="22" stopIfTrue="1">
       <formula>AND($D19="Med risk",J$5&gt;=$G19,J$5&lt;=$G19+$H19-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="38" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="42" priority="23" stopIfTrue="1">
       <formula>AND(LEN($D19)=0,J$5&gt;=$G19,J$5&lt;=$G19+$H19-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J19:BM19">
-    <cfRule type="expression" dxfId="37" priority="16">
+    <cfRule type="expression" dxfId="41" priority="16">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -42066,19 +42066,19 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J20:BM21">
-    <cfRule type="expression" dxfId="36" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="40" priority="11" stopIfTrue="1">
       <formula>AND($D20="Low risk",J$5&gt;=$G20,J$5&lt;=$G20+$H20-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="35" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="39" priority="12" stopIfTrue="1">
       <formula>AND($D20="High risk",J$5&gt;=$G20,J$5&lt;=$G20+$H20-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="38" priority="13" stopIfTrue="1">
       <formula>AND($D20="On track",J$5&gt;=$G20,J$5&lt;=$G20+$H20-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="37" priority="14" stopIfTrue="1">
       <formula>AND($D20="Med risk",J$5&gt;=$G20,J$5&lt;=$G20+$H20-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="36" priority="15" stopIfTrue="1">
       <formula>AND(LEN($D20)=0,J$5&gt;=$G20,J$5&lt;=$G20+$H20-1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -42097,7 +42097,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J20:GC21">
-    <cfRule type="expression" dxfId="31" priority="8">
+    <cfRule type="expression" dxfId="35" priority="8">
       <formula>AND(TODAY()&gt;=J$5,TODAY()&lt;K$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -42172,87 +42172,87 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J164:BM168">
-    <cfRule type="expression" dxfId="30" priority="430" stopIfTrue="1">
+    <cfRule type="expression" dxfId="34" priority="430" stopIfTrue="1">
       <formula>AND(#REF!="Low risk",J$5&gt;=$G164,J$5&lt;=$G164+$H164-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="431" stopIfTrue="1">
+    <cfRule type="expression" dxfId="33" priority="431" stopIfTrue="1">
       <formula>AND(#REF!="High risk",J$5&gt;=$G164,J$5&lt;=$G164+$H164-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="432" stopIfTrue="1">
+    <cfRule type="expression" dxfId="32" priority="432" stopIfTrue="1">
       <formula>AND(#REF!="On track",J$5&gt;=$G164,J$5&lt;=$G164+$H164-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="433" stopIfTrue="1">
+    <cfRule type="expression" dxfId="31" priority="433" stopIfTrue="1">
       <formula>AND(#REF!="Med risk",J$5&gt;=$G164,J$5&lt;=$G164+$H164-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="434" stopIfTrue="1">
+    <cfRule type="expression" dxfId="30" priority="434" stopIfTrue="1">
       <formula>AND(LEN(#REF!)=0,J$5&gt;=$G164,J$5&lt;=$G164+$H164-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J124:BM124">
-    <cfRule type="expression" dxfId="25" priority="501" stopIfTrue="1">
+    <cfRule type="expression" dxfId="29" priority="501" stopIfTrue="1">
       <formula>AND($D164="Low risk",J$5&gt;=$G124,J$5&lt;=$G124+$H124-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="502" stopIfTrue="1">
+    <cfRule type="expression" dxfId="28" priority="502" stopIfTrue="1">
       <formula>AND($D164="High risk",J$5&gt;=$G124,J$5&lt;=$G124+$H124-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="503" stopIfTrue="1">
+    <cfRule type="expression" dxfId="27" priority="503" stopIfTrue="1">
       <formula>AND($D164="On track",J$5&gt;=$G124,J$5&lt;=$G124+$H124-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="504" stopIfTrue="1">
+    <cfRule type="expression" dxfId="26" priority="504" stopIfTrue="1">
       <formula>AND($D164="Med risk",J$5&gt;=$G124,J$5&lt;=$G124+$H124-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="505" stopIfTrue="1">
+    <cfRule type="expression" dxfId="25" priority="505" stopIfTrue="1">
       <formula>AND(LEN($D164)=0,J$5&gt;=$G124,J$5&lt;=$G124+$H124-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J131:BM134">
-    <cfRule type="expression" dxfId="20" priority="781" stopIfTrue="1">
+    <cfRule type="expression" dxfId="24" priority="781" stopIfTrue="1">
       <formula>AND($D165="Low risk",J$5&gt;=$G131,J$5&lt;=$G131+$H131-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="782" stopIfTrue="1">
+    <cfRule type="expression" dxfId="23" priority="782" stopIfTrue="1">
       <formula>AND($D165="High risk",J$5&gt;=$G131,J$5&lt;=$G131+$H131-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="783" stopIfTrue="1">
+    <cfRule type="expression" dxfId="22" priority="783" stopIfTrue="1">
       <formula>AND($D165="On track",J$5&gt;=$G131,J$5&lt;=$G131+$H131-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="784" stopIfTrue="1">
+    <cfRule type="expression" dxfId="21" priority="784" stopIfTrue="1">
       <formula>AND($D165="Med risk",J$5&gt;=$G131,J$5&lt;=$G131+$H131-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="785" stopIfTrue="1">
+    <cfRule type="expression" dxfId="20" priority="785" stopIfTrue="1">
       <formula>AND(LEN($D165)=0,J$5&gt;=$G131,J$5&lt;=$G131+$H131-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J127:BM130">
-    <cfRule type="expression" dxfId="15" priority="796" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="796" stopIfTrue="1">
       <formula>AND($D162="Low risk",J$5&gt;=$G127,J$5&lt;=$G127+$H127-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="797" stopIfTrue="1">
+    <cfRule type="expression" dxfId="18" priority="797" stopIfTrue="1">
       <formula>AND($D162="High risk",J$5&gt;=$G127,J$5&lt;=$G127+$H127-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="798" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="798" stopIfTrue="1">
       <formula>AND($D162="On track",J$5&gt;=$G127,J$5&lt;=$G127+$H127-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="799" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="799" stopIfTrue="1">
       <formula>AND($D162="Med risk",J$5&gt;=$G127,J$5&lt;=$G127+$H127-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="800" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="800" stopIfTrue="1">
       <formula>AND(LEN($D162)=0,J$5&gt;=$G127,J$5&lt;=$G127+$H127-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J125:BM126">
-    <cfRule type="expression" dxfId="10" priority="823" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="823" stopIfTrue="1">
       <formula>AND($D161="Low risk",J$5&gt;=$G125,J$5&lt;=$G125+$H125-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="824" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="824" stopIfTrue="1">
       <formula>AND($D161="High risk",J$5&gt;=$G125,J$5&lt;=$G125+$H125-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="825" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="825" stopIfTrue="1">
       <formula>AND($D161="On track",J$5&gt;=$G125,J$5&lt;=$G125+$H125-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="826" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="826" stopIfTrue="1">
       <formula>AND($D161="Med risk",J$5&gt;=$G125,J$5&lt;=$G125+$H125-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="827" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="827" stopIfTrue="1">
       <formula>AND(LEN($D161)=0,J$5&gt;=$G125,J$5&lt;=$G125+$H125-1)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
some minnor fixes I notices added cookie policy and trigger
</commit_message>
<xml_diff>
--- a/Planning Report/application sprint planner sprint5 03.02.20.xlsx
+++ b/Planning Report/application sprint planner sprint5 03.02.20.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBEA7F44-23B1-4A6F-A8A4-9E310C899482}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F13D5043-6FA9-45DA-A6B3-6899AAE140E2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5520" yWindow="1050" windowWidth="21600" windowHeight="11385" tabRatio="415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2790" yWindow="690" windowWidth="21600" windowHeight="11385" tabRatio="415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gantt" sheetId="11" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="152">
   <si>
     <t>Create a Gantt Chart in this worksheet.
 Enter title of this project in cell B1. 
@@ -559,7 +559,7 @@
     <numFmt numFmtId="165" formatCode="d"/>
     <numFmt numFmtId="166" formatCode="#,##0_ ;\-#,##0\ "/>
   </numFmts>
-  <fonts count="34" x14ac:knownFonts="1">
+  <fonts count="35" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -800,6 +800,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="3" tint="-0.24994659260841701"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="3" tint="-0.24994659260841701"/>
       <name val="Calibri"/>
@@ -1345,7 +1353,7 @@
     <xf numFmtId="0" fontId="6" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1569,6 +1577,9 @@
     <xf numFmtId="0" fontId="18" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="50">
     <cellStyle name="20% - Accent1" xfId="28" builtinId="30" customBuiltin="1"/>
@@ -1636,10 +1647,38 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="2" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1668,34 +1707,6 @@
         </patternFill>
       </fill>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="2" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="2" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -4003,10 +4014,10 @@
     <filterColumn colId="6" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Milestone description" dataDxfId="9" totalsRowDxfId="8"/>
-    <tableColumn id="7" xr3:uid="{C2AA6DD8-DBD1-4E89-A1EF-3287225D3E74}" name="Required" dataDxfId="7" totalsRowDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Category" dataDxfId="5" totalsRowDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Estimated Duration" dataDxfId="3" totalsRowDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Milestone description" dataDxfId="9" totalsRowDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{C2AA6DD8-DBD1-4E89-A1EF-3287225D3E74}" name="Required" dataDxfId="8" totalsRowDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Category" dataDxfId="7" totalsRowDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Estimated Duration" dataDxfId="6" totalsRowDxfId="2"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Progress"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Start" totalsRowDxfId="1" dataCellStyle="Date"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="No. Days" totalsRowDxfId="0" dataCellStyle="Comma [0]"/>
@@ -4286,8 +4297,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:BM190"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A138" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="D149" sqref="D149"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A136" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="AU140" sqref="AU140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -28287,7 +28298,9 @@
     </row>
     <row r="122" spans="1:65" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="15"/>
-      <c r="B122" s="69"/>
+      <c r="B122" s="85" t="s">
+        <v>49</v>
+      </c>
       <c r="C122" s="53"/>
       <c r="D122" s="34"/>
       <c r="E122" s="34"/>
@@ -32228,13 +32241,19 @@
         <v>105</v>
       </c>
       <c r="C139" s="41"/>
-      <c r="D139" s="34"/>
+      <c r="D139" s="34" t="s">
+        <v>17</v>
+      </c>
       <c r="E139" s="34">
         <v>0.5</v>
       </c>
       <c r="F139" s="59"/>
-      <c r="G139" s="71"/>
-      <c r="H139" s="72"/>
+      <c r="G139" s="32">
+        <v>43892</v>
+      </c>
+      <c r="H139" s="72">
+        <v>1</v>
+      </c>
       <c r="I139" s="26"/>
       <c r="J139" s="38" t="str">
         <f t="shared" ca="1" si="82"/>
@@ -33184,13 +33203,19 @@
         <v>151</v>
       </c>
       <c r="C143" s="41"/>
-      <c r="D143" s="34"/>
+      <c r="D143" s="34" t="s">
+        <v>17</v>
+      </c>
       <c r="E143" s="34">
         <v>2</v>
       </c>
       <c r="F143" s="59"/>
-      <c r="G143" s="71"/>
-      <c r="H143" s="72"/>
+      <c r="G143" s="32">
+        <v>43895</v>
+      </c>
+      <c r="H143" s="72">
+        <v>1</v>
+      </c>
       <c r="I143" s="26"/>
       <c r="J143" s="38" t="str">
         <f t="shared" ca="1" si="82"/>
@@ -33423,13 +33448,19 @@
         <v>133</v>
       </c>
       <c r="C144" s="41"/>
-      <c r="D144" s="34"/>
+      <c r="D144" s="34" t="s">
+        <v>17</v>
+      </c>
       <c r="E144" s="34">
         <v>3</v>
       </c>
       <c r="F144" s="59"/>
-      <c r="G144" s="71"/>
-      <c r="H144" s="72"/>
+      <c r="G144" s="71">
+        <v>43899</v>
+      </c>
+      <c r="H144" s="72">
+        <v>1</v>
+      </c>
       <c r="I144" s="26"/>
       <c r="J144" s="38" t="str">
         <f t="shared" ca="1" si="82"/>
@@ -33662,13 +33693,19 @@
         <v>148</v>
       </c>
       <c r="C145" s="41"/>
-      <c r="D145" s="34"/>
+      <c r="D145" s="34" t="s">
+        <v>17</v>
+      </c>
       <c r="E145" s="34">
         <v>6</v>
       </c>
       <c r="F145" s="59"/>
-      <c r="G145" s="71"/>
-      <c r="H145" s="72"/>
+      <c r="G145" s="32">
+        <v>43893</v>
+      </c>
+      <c r="H145" s="72">
+        <v>1</v>
+      </c>
       <c r="I145" s="26"/>
       <c r="J145" s="38" t="str">
         <f t="shared" ca="1" si="82"/>
@@ -33901,13 +33938,19 @@
         <v>147</v>
       </c>
       <c r="C146" s="41"/>
-      <c r="D146" s="34"/>
+      <c r="D146" s="34" t="s">
+        <v>17</v>
+      </c>
       <c r="E146" s="34">
         <v>2</v>
       </c>
       <c r="F146" s="59"/>
-      <c r="G146" s="71"/>
-      <c r="H146" s="72"/>
+      <c r="G146" s="32">
+        <v>43893</v>
+      </c>
+      <c r="H146" s="72">
+        <v>1</v>
+      </c>
       <c r="I146" s="26"/>
       <c r="J146" s="38" t="str">
         <f t="shared" ca="1" si="82"/>
@@ -34379,13 +34422,19 @@
         <v>48</v>
       </c>
       <c r="C148" s="41"/>
-      <c r="D148" s="34"/>
+      <c r="D148" s="34" t="s">
+        <v>17</v>
+      </c>
       <c r="E148" s="34">
         <v>2</v>
       </c>
       <c r="F148" s="59"/>
-      <c r="G148" s="71"/>
-      <c r="H148" s="72"/>
+      <c r="G148" s="32">
+        <v>43895</v>
+      </c>
+      <c r="H148" s="72">
+        <v>1</v>
+      </c>
       <c r="I148" s="26"/>
       <c r="J148" s="38" t="str">
         <f t="shared" ca="1" si="82"/>
@@ -35333,7 +35382,7 @@
       <c r="E152" s="34"/>
       <c r="F152" s="31"/>
       <c r="G152" s="32">
-        <v>43922</v>
+        <v>43920</v>
       </c>
       <c r="H152" s="33">
         <v>14</v>
@@ -35574,7 +35623,7 @@
       <c r="E153" s="34"/>
       <c r="F153" s="31"/>
       <c r="G153" s="32">
-        <v>43927</v>
+        <v>43934</v>
       </c>
       <c r="H153" s="33">
         <v>14</v>

</xml_diff>

<commit_message>
document changes to allow for edit team and add tasks permissions
</commit_message>
<xml_diff>
--- a/Planning Report/application sprint planner sprint5 03.02.20.xlsx
+++ b/Planning Report/application sprint planner sprint5 03.02.20.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F13D5043-6FA9-45DA-A6B3-6899AAE140E2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F5D59B2-CF20-401C-8241-6F8775B911B6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2790" yWindow="690" windowWidth="21600" windowHeight="11385" tabRatio="415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29580" yWindow="780" windowWidth="21600" windowHeight="11385" tabRatio="415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gantt" sheetId="11" r:id="rId1"/>
@@ -1549,6 +1549,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1576,9 +1579,6 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="50">
@@ -1647,6 +1647,12 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1675,15 +1681,6 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="2" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -1707,6 +1704,9 @@
         </patternFill>
       </fill>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="2" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -4014,10 +4014,10 @@
     <filterColumn colId="6" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Milestone description" dataDxfId="9" totalsRowDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{C2AA6DD8-DBD1-4E89-A1EF-3287225D3E74}" name="Required" dataDxfId="8" totalsRowDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Category" dataDxfId="7" totalsRowDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Estimated Duration" dataDxfId="6" totalsRowDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Milestone description" dataDxfId="9" totalsRowDxfId="8"/>
+    <tableColumn id="7" xr3:uid="{C2AA6DD8-DBD1-4E89-A1EF-3287225D3E74}" name="Required" dataDxfId="7" totalsRowDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Category" dataDxfId="5" totalsRowDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Estimated Duration" dataDxfId="3" totalsRowDxfId="2"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Progress"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Start" totalsRowDxfId="1" dataCellStyle="Date"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="No. Days" totalsRowDxfId="0" dataCellStyle="Comma [0]"/>
@@ -4297,8 +4297,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:BM190"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A136" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="AU140" sqref="AU140"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A142" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="AX142" sqref="AX142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4367,39 +4367,39 @@
       <c r="D2" s="18"/>
       <c r="G2" s="23"/>
       <c r="H2" s="21"/>
-      <c r="J2" s="82" t="s">
+      <c r="J2" s="83" t="s">
         <v>20</v>
       </c>
-      <c r="K2" s="82"/>
-      <c r="L2" s="82"/>
-      <c r="M2" s="82"/>
-      <c r="O2" s="83" t="s">
+      <c r="K2" s="83"/>
+      <c r="L2" s="83"/>
+      <c r="M2" s="83"/>
+      <c r="O2" s="84" t="s">
         <v>17</v>
       </c>
-      <c r="P2" s="83"/>
-      <c r="Q2" s="83"/>
-      <c r="R2" s="83"/>
+      <c r="P2" s="84"/>
+      <c r="Q2" s="84"/>
+      <c r="R2" s="84"/>
       <c r="S2" s="20"/>
-      <c r="T2" s="84" t="s">
+      <c r="T2" s="85" t="s">
         <v>18</v>
       </c>
-      <c r="U2" s="84"/>
-      <c r="V2" s="84"/>
-      <c r="W2" s="84"/>
+      <c r="U2" s="85"/>
+      <c r="V2" s="85"/>
+      <c r="W2" s="85"/>
       <c r="X2" s="20"/>
-      <c r="Y2" s="75" t="s">
+      <c r="Y2" s="76" t="s">
         <v>19</v>
       </c>
-      <c r="Z2" s="75"/>
-      <c r="AA2" s="75"/>
-      <c r="AB2" s="75"/>
+      <c r="Z2" s="76"/>
+      <c r="AA2" s="76"/>
+      <c r="AB2" s="76"/>
       <c r="AC2" s="20"/>
-      <c r="AD2" s="76" t="s">
+      <c r="AD2" s="77" t="s">
         <v>27</v>
       </c>
-      <c r="AE2" s="76"/>
-      <c r="AF2" s="76"/>
-      <c r="AG2" s="76"/>
+      <c r="AE2" s="77"/>
+      <c r="AF2" s="77"/>
+      <c r="AG2" s="77"/>
     </row>
     <row r="3" spans="1:65" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
@@ -4410,25 +4410,25 @@
       </c>
       <c r="C3" s="19"/>
       <c r="D3" s="19"/>
-      <c r="E3" s="77" t="s">
+      <c r="E3" s="78" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="78"/>
-      <c r="G3" s="80">
+      <c r="F3" s="79"/>
+      <c r="G3" s="81">
         <f ca="1">IFERROR(IF(MIN(Milestones[Start])=0,TODAY(),MIN(Milestones[Start])),TODAY())</f>
         <v>43773</v>
       </c>
-      <c r="H3" s="81"/>
+      <c r="H3" s="82"/>
       <c r="I3" s="22"/>
     </row>
     <row r="4" spans="1:65" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="77" t="s">
+      <c r="E4" s="78" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="78"/>
+      <c r="F4" s="79"/>
       <c r="G4" s="44">
         <v>85</v>
       </c>
@@ -4517,14 +4517,14 @@
       <c r="A5" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="79"/>
-      <c r="C5" s="79"/>
-      <c r="D5" s="79"/>
-      <c r="E5" s="79"/>
-      <c r="F5" s="79"/>
-      <c r="G5" s="79"/>
-      <c r="H5" s="79"/>
-      <c r="I5" s="79"/>
+      <c r="B5" s="80"/>
+      <c r="C5" s="80"/>
+      <c r="D5" s="80"/>
+      <c r="E5" s="80"/>
+      <c r="F5" s="80"/>
+      <c r="G5" s="80"/>
+      <c r="H5" s="80"/>
+      <c r="I5" s="80"/>
       <c r="J5" s="46">
         <f ca="1">IFERROR(Project_Start+Scrolling_Increment,TODAY())</f>
         <v>43858</v>
@@ -28298,7 +28298,7 @@
     </row>
     <row r="122" spans="1:65" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="15"/>
-      <c r="B122" s="85" t="s">
+      <c r="B122" s="75" t="s">
         <v>49</v>
       </c>
       <c r="C122" s="53"/>

</xml_diff>

<commit_message>
changes to invite code button position and css text shadows
</commit_message>
<xml_diff>
--- a/Planning Report/application sprint planner sprint5 03.02.20.xlsx
+++ b/Planning Report/application sprint planner sprint5 03.02.20.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F5D59B2-CF20-401C-8241-6F8775B911B6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E3DE43E-FC6C-4081-B5A1-7A6A255E172C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29580" yWindow="780" windowWidth="21600" windowHeight="11385" tabRatio="415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gantt" sheetId="11" r:id="rId1"/>
@@ -1647,10 +1647,38 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="2" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1679,34 +1707,6 @@
         </patternFill>
       </fill>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="2" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="2" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -4014,10 +4014,10 @@
     <filterColumn colId="6" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Milestone description" dataDxfId="9" totalsRowDxfId="8"/>
-    <tableColumn id="7" xr3:uid="{C2AA6DD8-DBD1-4E89-A1EF-3287225D3E74}" name="Required" dataDxfId="7" totalsRowDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Category" dataDxfId="5" totalsRowDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Estimated Duration" dataDxfId="3" totalsRowDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Milestone description" dataDxfId="9" totalsRowDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{C2AA6DD8-DBD1-4E89-A1EF-3287225D3E74}" name="Required" dataDxfId="8" totalsRowDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Category" dataDxfId="7" totalsRowDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Estimated Duration" dataDxfId="6" totalsRowDxfId="2"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Progress"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Start" totalsRowDxfId="1" dataCellStyle="Date"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="No. Days" totalsRowDxfId="0" dataCellStyle="Comma [0]"/>
@@ -4297,8 +4297,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:BM190"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A142" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="AX142" sqref="AX142"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A136" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="AF140" sqref="AF140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -32969,8 +32969,12 @@
         <v>4</v>
       </c>
       <c r="F142" s="59"/>
-      <c r="G142" s="71"/>
-      <c r="H142" s="72"/>
+      <c r="G142" s="71">
+        <v>43899</v>
+      </c>
+      <c r="H142" s="72">
+        <v>1</v>
+      </c>
       <c r="I142" s="26"/>
       <c r="J142" s="38" t="str">
         <f t="shared" ca="1" si="82"/>

</xml_diff>

<commit_message>
significant document changes fixed issue with levelup notification
</commit_message>
<xml_diff>
--- a/Planning Report/application sprint planner sprint5 03.02.20.xlsx
+++ b/Planning Report/application sprint planner sprint5 03.02.20.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ACE1DA7-740A-4AAF-92EB-D9D4E765975E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E6FDDC1-CEB3-4911-8B51-92EC19EBE044}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3270" yWindow="0" windowWidth="21600" windowHeight="11385" tabRatio="415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gantt" sheetId="11" r:id="rId1"/>
@@ -1662,6 +1662,12 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1690,15 +1696,6 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="2" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -1722,6 +1719,9 @@
         </patternFill>
       </fill>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="2" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -4012,10 +4012,10 @@
     <filterColumn colId="6" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Milestone description" dataDxfId="9" totalsRowDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{C2AA6DD8-DBD1-4E89-A1EF-3287225D3E74}" name="Required" dataDxfId="8" totalsRowDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Category" dataDxfId="7" totalsRowDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Estimated Duration" dataDxfId="6" totalsRowDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Milestone description" dataDxfId="9" totalsRowDxfId="8"/>
+    <tableColumn id="7" xr3:uid="{C2AA6DD8-DBD1-4E89-A1EF-3287225D3E74}" name="Required" dataDxfId="7" totalsRowDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Category" dataDxfId="5" totalsRowDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Estimated Duration" dataDxfId="3" totalsRowDxfId="2"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Progress"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Start" totalsRowDxfId="1" dataCellStyle="Date"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="No. Days" totalsRowDxfId="0" dataCellStyle="Comma [0]"/>
@@ -4295,8 +4295,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:BM202"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A136" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="AF149" sqref="AF149"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A154" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="AA163" sqref="AA163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>